<commit_message>
Edited componentOwnership doc, edited unit test file a smidgen. Quietly, embarassingly realising I need to ask for an extension.
</commit_message>
<xml_diff>
--- a/componentOwnership.xlsx
+++ b/componentOwnership.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\PycharmProjects\Python2UML\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EA121B1-DE21-474B-967F-5223F5883926}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-4740" yWindow="6990" windowWidth="11535" windowHeight="12405" xr2:uid="{93F002C3-555C-427F-849D-0EA0A5F8013E}"/>
+    <workbookView xWindow="-4740" yWindow="6990" windowWidth="11535" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>Features</t>
   </si>
@@ -97,12 +91,33 @@
   </si>
   <si>
     <t>Can raise exceptions and provide exception handling</t>
+  </si>
+  <si>
+    <t>Amount of checking for pre- and post- conditions of methods</t>
+  </si>
+  <si>
+    <t>Provide doctests</t>
+  </si>
+  <si>
+    <t>Provide unittests</t>
+  </si>
+  <si>
+    <t>Pretty print, i.e., displaying data in chart/ diagram, etc.</t>
+  </si>
+  <si>
+    <t>Can save and read data from a database, e.g., SQLite, MySQL and MongoDB</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>0-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -194,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -246,7 +261,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -440,18 +455,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36731647-B863-4A49-98D1-DF30D9CDDFFF}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +476,7 @@
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +486,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -482,8 +500,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -493,8 +514,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -504,8 +528,11 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -515,8 +542,11 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -526,8 +556,11 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -537,8 +570,11 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -548,8 +584,11 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -559,8 +598,11 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -570,13 +612,59 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a bug with saveConfig not respecting the given path.
</commit_message>
<xml_diff>
--- a/componentOwnership.xlsx
+++ b/componentOwnership.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\PycharmProjects\Python2UML\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC379D1-76B3-4300-B963-D815034079B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Features</t>
   </si>
@@ -118,12 +112,18 @@
   </si>
   <si>
     <t>commandLine.py</t>
+  </si>
+  <si>
+    <t>database.py</t>
+  </si>
+  <si>
+    <t>pieChart.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,18 +461,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,8 +673,11 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -683,6 +686,9 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>

</xml_diff>